<commit_message>
updated calibration and shell of lab 4
</commit_message>
<xml_diff>
--- a/Data-Lab03/Sensor calibration data.xlsx
+++ b/Data-Lab03/Sensor calibration data.xlsx
@@ -319,11 +319,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61806848"/>
-        <c:axId val="61812736"/>
+        <c:axId val="109775104"/>
+        <c:axId val="109780992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61806848"/>
+        <c:axId val="109775104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -333,12 +333,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61812736"/>
+        <c:crossAx val="109780992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61812736"/>
+        <c:axId val="109780992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -349,7 +349,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61806848"/>
+        <c:crossAx val="109775104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -394,122 +394,154 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.27168503937007876"/>
+                  <c:y val="-7.2116141732283465E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'IR sensor'!$A$5:$A$21</c:f>
+              <c:f>'Sonar sensor'!$B$25:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>248</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>445</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>520</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11</c:v>
+                  <c:v>776</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>880</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13</c:v>
+                  <c:v>962</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14</c:v>
+                  <c:v>1050</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15</c:v>
+                  <c:v>1138</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16</c:v>
+                  <c:v>1227</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17</c:v>
+                  <c:v>1312</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18</c:v>
+                  <c:v>1405</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>19</c:v>
+                  <c:v>1509</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20</c:v>
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1680</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1798</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IR sensor'!$B$5:$B$21</c:f>
+              <c:f>'Sonar sensor'!$A$25:$A$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>454</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>380</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>327</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>283</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>253</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>229</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>214</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>198</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>185</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>171</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>161</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>150</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>138</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>131</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>122</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>126</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>121</c:v>
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -524,11 +556,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64507904"/>
-        <c:axId val="64509440"/>
+        <c:axId val="52206208"/>
+        <c:axId val="52204672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64507904"/>
+        <c:axId val="52206208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -538,12 +570,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64509440"/>
+        <c:crossAx val="52204672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64509440"/>
+        <c:axId val="52204672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -554,7 +586,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64507904"/>
+        <c:crossAx val="52206208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -572,6 +604,211 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'IR sensor'!$A$5:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'IR sensor'!$B$5:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>454</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>283</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>121</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="109858816"/>
+        <c:axId val="109860352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="109858816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="109860352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="109860352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="109858816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -743,11 +980,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64534016"/>
-        <c:axId val="64535552"/>
+        <c:axId val="109880832"/>
+        <c:axId val="109882368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64534016"/>
+        <c:axId val="109880832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -757,12 +994,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64535552"/>
+        <c:crossAx val="109882368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64535552"/>
+        <c:axId val="109882368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -773,7 +1010,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64534016"/>
+        <c:crossAx val="109880832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -790,7 +1027,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -966,11 +1203,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="67398272"/>
-        <c:axId val="67400064"/>
+        <c:axId val="110312064"/>
+        <c:axId val="110313856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67398272"/>
+        <c:axId val="110312064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -980,12 +1217,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67400064"/>
+        <c:crossAx val="110313856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67400064"/>
+        <c:axId val="110313856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -996,7 +1233,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67398272"/>
+        <c:crossAx val="110312064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1040,6 +1277,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1435,17 +1702,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1458,7 +1725,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1780,6 +2047,326 @@
       <c r="D21" s="2">
         <f t="shared" si="1"/>
         <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>162</v>
+      </c>
+      <c r="C25">
+        <f>0.0111*B25-0.8107</f>
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="D25" s="2">
+        <f>ABS(A25-C25)/A25</f>
+        <v>1.2499999999999956E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>248</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:C44" si="2">0.0111*B26-0.8107</f>
+        <v>1.9421000000000002</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" ref="D26:D44" si="3">ABS(A26-C26)/A26</f>
+        <v>2.894999999999992E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>360</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="2"/>
+        <v>3.1852999999999998</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="3"/>
+        <v>6.1766666666666602E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>445</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>4.1288</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="3"/>
+        <v>3.2200000000000006E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>520</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>4.9613000000000005</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="3"/>
+        <v>7.7399999999999023E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>630</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>6.1823000000000006</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="3"/>
+        <v>3.0383333333333429E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>700</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>6.9593000000000007</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="3"/>
+        <v>5.8142857142856131E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>776</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>7.8029000000000002</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="3"/>
+        <v>2.4637499999999979E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>880</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>8.9573</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="3"/>
+        <v>4.74444444444444E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>962</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>9.8674999999999997</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="3"/>
+        <v>1.3250000000000029E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <v>1050</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>10.8443</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="3"/>
+        <v>1.4154545454545409E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>12</v>
+      </c>
+      <c r="B36">
+        <v>1138</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>11.821099999999999</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="3"/>
+        <v>1.4908333333333376E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>13</v>
+      </c>
+      <c r="B37">
+        <v>1227</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>12.808999999999999</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="3"/>
+        <v>1.4692307692307748E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>14</v>
+      </c>
+      <c r="B38">
+        <v>1312</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>13.7525</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" si="3"/>
+        <v>1.7678571428571464E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>15</v>
+      </c>
+      <c r="B39">
+        <v>1405</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>14.784800000000001</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="3"/>
+        <v>1.4346666666666626E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>16</v>
+      </c>
+      <c r="B40">
+        <v>1509</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="2"/>
+        <v>15.9392</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="3"/>
+        <v>3.8000000000000256E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>17</v>
+      </c>
+      <c r="B41">
+        <v>1600</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="2"/>
+        <v>16.949300000000001</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="3"/>
+        <v>2.9823529411764165E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>18</v>
+      </c>
+      <c r="B42">
+        <v>1680</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="2"/>
+        <v>17.837299999999999</v>
+      </c>
+      <c r="D42" s="2">
+        <f t="shared" si="3"/>
+        <v>9.0388888888889417E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>19</v>
+      </c>
+      <c r="B43">
+        <v>1798</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="2"/>
+        <v>19.147100000000002</v>
+      </c>
+      <c r="D43" s="2">
+        <f t="shared" si="3"/>
+        <v>7.7421052631579884E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>20</v>
+      </c>
+      <c r="B44">
+        <v>1889</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="2"/>
+        <v>20.1572</v>
+      </c>
+      <c r="D44" s="2">
+        <f t="shared" si="3"/>
+        <v>7.8599999999999781E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>